<commit_message>
t tests aggregate data
</commit_message>
<xml_diff>
--- a/data/out/kaggle/fifa/standings_wc_fifa_men.xlsx
+++ b/data/out/kaggle/fifa/standings_wc_fifa_men.xlsx
@@ -522,7 +522,7 @@
       <c r="G2" t="inlineStr"/>
       <c r="H2" t="inlineStr">
         <is>
-          <t>['Italy', 'Argentina', 'Bulgaria']</t>
+          <t>['Argentina', 'Italy', 'Bulgaria']</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -571,7 +571,7 @@
       <c r="G3" t="inlineStr"/>
       <c r="H3" t="inlineStr">
         <is>
-          <t>['Belgium', 'Mexico', 'Paraguay']</t>
+          <t>['Mexico', 'Paraguay', 'Belgium']</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -669,7 +669,7 @@
       <c r="G5" t="inlineStr"/>
       <c r="H5" t="inlineStr">
         <is>
-          <t>['Northern Ireland', 'Spain', 'Brazil']</t>
+          <t>['Northern Ireland', 'Brazil', 'Spain']</t>
         </is>
       </c>
       <c r="I5" t="inlineStr">
@@ -728,7 +728,7 @@
       </c>
       <c r="H6" t="inlineStr">
         <is>
-          <t>['Algeria', 'Spain', 'Brazil']</t>
+          <t>['Algeria', 'Brazil', 'Spain']</t>
         </is>
       </c>
       <c r="I6" t="inlineStr">
@@ -787,7 +787,7 @@
       </c>
       <c r="H7" t="inlineStr">
         <is>
-          <t>['Northern Ireland', 'Spain', 'Brazil']</t>
+          <t>['Northern Ireland', 'Brazil', 'Spain']</t>
         </is>
       </c>
       <c r="I7" t="inlineStr">
@@ -836,7 +836,7 @@
       <c r="G8" t="inlineStr"/>
       <c r="H8" t="inlineStr">
         <is>
-          <t>['Denmark', 'Uruguay', 'West Germany']</t>
+          <t>['Uruguay', 'Denmark', 'West Germany']</t>
         </is>
       </c>
       <c r="I8" t="inlineStr">
@@ -885,7 +885,7 @@
       <c r="G9" t="inlineStr"/>
       <c r="H9" t="inlineStr">
         <is>
-          <t>['Poland', 'Portugal', 'Morocco']</t>
+          <t>['Portugal', 'Morocco', 'Poland']</t>
         </is>
       </c>
       <c r="I9" t="inlineStr">
@@ -944,7 +944,7 @@
       </c>
       <c r="H10" t="inlineStr">
         <is>
-          <t>['Poland', 'Portugal', 'England']</t>
+          <t>['Portugal', 'England', 'Poland']</t>
         </is>
       </c>
       <c r="I10" t="inlineStr">
@@ -1003,7 +1003,7 @@
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>['Portugal', 'England', 'Morocco']</t>
+          <t>['Portugal', 'Morocco', 'England']</t>
         </is>
       </c>
       <c r="I11" t="inlineStr">
@@ -1062,7 +1062,7 @@
       </c>
       <c r="H12" t="inlineStr">
         <is>
-          <t>['Poland', 'England', 'Morocco']</t>
+          <t>['Morocco', 'England', 'Poland']</t>
         </is>
       </c>
       <c r="I12" t="inlineStr">
@@ -1111,7 +1111,7 @@
       <c r="G13" t="inlineStr"/>
       <c r="H13" t="inlineStr">
         <is>
-          <t>['Czechoslovakia', 'Italy', 'Austria']</t>
+          <t>['Italy', 'Czechoslovakia', 'Austria']</t>
         </is>
       </c>
       <c r="I13" t="inlineStr">
@@ -1160,7 +1160,7 @@
       <c r="G14" t="inlineStr"/>
       <c r="H14" t="inlineStr">
         <is>
-          <t>['Romania', 'Argentina', 'Cameroon']</t>
+          <t>['Argentina', 'Romania', 'Cameroon']</t>
         </is>
       </c>
       <c r="I14" t="inlineStr">
@@ -1219,7 +1219,7 @@
       </c>
       <c r="H15" t="inlineStr">
         <is>
-          <t>['Soviet Union', 'Argentina', 'Cameroon']</t>
+          <t>['Argentina', 'Soviet Union', 'Cameroon']</t>
         </is>
       </c>
       <c r="I15" t="inlineStr">
@@ -1278,7 +1278,7 @@
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>['Romania', 'Argentina', 'Cameroon']</t>
+          <t>['Argentina', 'Romania', 'Cameroon']</t>
         </is>
       </c>
       <c r="I16" t="inlineStr">
@@ -1327,7 +1327,7 @@
       <c r="G17" t="inlineStr"/>
       <c r="H17" t="inlineStr">
         <is>
-          <t>['Scotland', 'Brazil', 'Costa Rica']</t>
+          <t>['Costa Rica', 'Scotland', 'Brazil']</t>
         </is>
       </c>
       <c r="I17" t="inlineStr">
@@ -1445,7 +1445,7 @@
       </c>
       <c r="H19" t="inlineStr">
         <is>
-          <t>['Scotland', 'Brazil', 'Costa Rica']</t>
+          <t>['Costa Rica', 'Scotland', 'Brazil']</t>
         </is>
       </c>
       <c r="I19" t="inlineStr">
@@ -1494,7 +1494,7 @@
       <c r="G20" t="inlineStr"/>
       <c r="H20" t="inlineStr">
         <is>
-          <t>['Colombia', 'West Germany', 'Yugoslavia']</t>
+          <t>['Yugoslavia', 'Colombia', 'West Germany']</t>
         </is>
       </c>
       <c r="I20" t="inlineStr">
@@ -1543,7 +1543,7 @@
       <c r="G21" t="inlineStr"/>
       <c r="H21" t="inlineStr">
         <is>
-          <t>['Belgium', 'Spain', 'Uruguay']</t>
+          <t>['Belgium', 'Uruguay', 'Spain']</t>
         </is>
       </c>
       <c r="I21" t="inlineStr">
@@ -1592,7 +1592,7 @@
       <c r="G22" t="inlineStr"/>
       <c r="H22" t="inlineStr">
         <is>
-          <t>['Republic of Ireland', 'England', 'Netherlands']</t>
+          <t>['Netherlands', 'England', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="I22" t="inlineStr">
@@ -1651,7 +1651,7 @@
       </c>
       <c r="H23" t="inlineStr">
         <is>
-          <t>['Egypt', 'England', 'Netherlands']</t>
+          <t>['Egypt', 'Netherlands', 'England']</t>
         </is>
       </c>
       <c r="I23" t="inlineStr">
@@ -1710,7 +1710,7 @@
       </c>
       <c r="H24" t="inlineStr">
         <is>
-          <t>['Republic of Ireland', 'England', 'Netherlands']</t>
+          <t>['Netherlands', 'England', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="I24" t="inlineStr">
@@ -1759,7 +1759,7 @@
       <c r="G25" t="inlineStr"/>
       <c r="H25" t="inlineStr">
         <is>
-          <t>['Romania', 'United States', 'Switzerland']</t>
+          <t>['United States', 'Switzerland', 'Romania']</t>
         </is>
       </c>
       <c r="I25" t="inlineStr">
@@ -1867,7 +1867,7 @@
       </c>
       <c r="H27" t="inlineStr">
         <is>
-          <t>['Sweden', 'Brazil', 'Russia']</t>
+          <t>['Sweden', 'Russia', 'Brazil']</t>
         </is>
       </c>
       <c r="I27" t="inlineStr">
@@ -1916,7 +1916,7 @@
       <c r="G28" t="inlineStr"/>
       <c r="H28" t="inlineStr">
         <is>
-          <t>['South Korea', 'Spain', 'Germany']</t>
+          <t>['Germany', 'South Korea', 'Spain']</t>
         </is>
       </c>
       <c r="I28" t="inlineStr">
@@ -1965,7 +1965,7 @@
       <c r="G29" t="inlineStr"/>
       <c r="H29" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina', 'Bulgaria']</t>
+          <t>['Argentina', 'Nigeria', 'Bulgaria']</t>
         </is>
       </c>
       <c r="I29" t="inlineStr">
@@ -2014,7 +2014,7 @@
       <c r="G30" t="inlineStr"/>
       <c r="H30" t="inlineStr">
         <is>
-          <t>['Republic of Ireland', 'Mexico', 'Italy']</t>
+          <t>['Mexico', 'Italy', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="I30" t="inlineStr">
@@ -2073,7 +2073,7 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>['Norway', 'Republic of Ireland', 'Italy']</t>
+          <t>['Norway', 'Italy', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
@@ -2132,7 +2132,7 @@
       </c>
       <c r="H32" t="inlineStr">
         <is>
-          <t>['Republic of Ireland', 'Mexico', 'Italy']</t>
+          <t>['Mexico', 'Italy', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="I32" t="inlineStr">
@@ -2289,7 +2289,7 @@
       </c>
       <c r="H35" t="inlineStr">
         <is>
-          <t>['Brazil', 'Morocco']</t>
+          <t>['Morocco', 'Brazil']</t>
         </is>
       </c>
       <c r="I35" t="inlineStr">
@@ -2397,7 +2397,7 @@
       <c r="G37" t="inlineStr"/>
       <c r="H37" t="inlineStr">
         <is>
-          <t>['Italy', 'Chile']</t>
+          <t>['Chile', 'Italy']</t>
         </is>
       </c>
       <c r="I37" t="inlineStr">
@@ -2554,7 +2554,7 @@
       </c>
       <c r="H40" t="inlineStr">
         <is>
-          <t>['Spain', 'Nigeria']</t>
+          <t>['Nigeria', 'Spain']</t>
         </is>
       </c>
       <c r="I40" t="inlineStr">
@@ -2662,7 +2662,7 @@
       <c r="G42" t="inlineStr"/>
       <c r="H42" t="inlineStr">
         <is>
-          <t>['Mexico', 'Netherlands']</t>
+          <t>['Netherlands', 'Mexico']</t>
         </is>
       </c>
       <c r="I42" t="inlineStr">
@@ -2721,7 +2721,7 @@
       </c>
       <c r="H43" t="inlineStr">
         <is>
-          <t>['Belgium', 'Netherlands']</t>
+          <t>['Netherlands', 'Belgium']</t>
         </is>
       </c>
       <c r="I43" t="inlineStr">
@@ -2780,7 +2780,7 @@
       </c>
       <c r="H44" t="inlineStr">
         <is>
-          <t>['Mexico', 'Netherlands']</t>
+          <t>['Netherlands', 'Mexico']</t>
         </is>
       </c>
       <c r="I44" t="inlineStr">
@@ -2927,7 +2927,7 @@
       <c r="G47" t="inlineStr"/>
       <c r="H47" t="inlineStr">
         <is>
-          <t>['Croatia', 'Argentina']</t>
+          <t>['Argentina', 'Croatia']</t>
         </is>
       </c>
       <c r="I47" t="inlineStr">
@@ -2976,7 +2976,7 @@
       <c r="G48" t="inlineStr"/>
       <c r="H48" t="inlineStr">
         <is>
-          <t>['Denmark', 'Senegal']</t>
+          <t>['Senegal', 'Denmark']</t>
         </is>
       </c>
       <c r="I48" t="inlineStr">
@@ -3084,7 +3084,7 @@
       </c>
       <c r="H50" t="inlineStr">
         <is>
-          <t>['Spain', 'Paraguay']</t>
+          <t>['Paraguay', 'Spain']</t>
         </is>
       </c>
       <c r="I50" t="inlineStr">
@@ -3133,7 +3133,7 @@
       <c r="G51" t="inlineStr"/>
       <c r="H51" t="inlineStr">
         <is>
-          <t>['Brazil', 'Costa Rica']</t>
+          <t>['Costa Rica', 'Brazil']</t>
         </is>
       </c>
       <c r="I51" t="inlineStr">
@@ -3192,7 +3192,7 @@
       </c>
       <c r="H52" t="inlineStr">
         <is>
-          <t>['Brazil', 'Turkey']</t>
+          <t>['Turkey', 'Brazil']</t>
         </is>
       </c>
       <c r="I52" t="inlineStr">
@@ -3251,7 +3251,7 @@
       </c>
       <c r="H53" t="inlineStr">
         <is>
-          <t>['Brazil', 'Costa Rica']</t>
+          <t>['Costa Rica', 'Brazil']</t>
         </is>
       </c>
       <c r="I53" t="inlineStr">
@@ -3310,7 +3310,7 @@
       </c>
       <c r="H54" t="inlineStr">
         <is>
-          <t>['Brazil', 'Turkey']</t>
+          <t>['Turkey', 'Brazil']</t>
         </is>
       </c>
       <c r="I54" t="inlineStr">
@@ -3359,7 +3359,7 @@
       <c r="G55" t="inlineStr"/>
       <c r="H55" t="inlineStr">
         <is>
-          <t>['South Korea', 'United States']</t>
+          <t>['United States', 'South Korea']</t>
         </is>
       </c>
       <c r="I55" t="inlineStr">
@@ -3477,7 +3477,7 @@
       </c>
       <c r="H57" t="inlineStr">
         <is>
-          <t>['South Korea', 'United States']</t>
+          <t>['United States', 'South Korea']</t>
         </is>
       </c>
       <c r="I57" t="inlineStr">
@@ -3585,7 +3585,7 @@
       </c>
       <c r="H59" t="inlineStr">
         <is>
-          <t>['Republic of Ireland', 'Germany']</t>
+          <t>['Germany', 'Republic of Ireland']</t>
         </is>
       </c>
       <c r="I59" t="inlineStr">
@@ -3850,7 +3850,7 @@
       <c r="G64" t="inlineStr"/>
       <c r="H64" t="inlineStr">
         <is>
-          <t>['Japan', 'Russia']</t>
+          <t>['Russia', 'Japan']</t>
         </is>
       </c>
       <c r="I64" t="inlineStr">
@@ -3909,7 +3909,7 @@
       </c>
       <c r="H65" t="inlineStr">
         <is>
-          <t>['Japan', 'Belgium']</t>
+          <t>['Belgium', 'Japan']</t>
         </is>
       </c>
       <c r="I65" t="inlineStr">
@@ -3968,7 +3968,7 @@
       </c>
       <c r="H66" t="inlineStr">
         <is>
-          <t>['Japan', 'Russia']</t>
+          <t>['Russia', 'Japan']</t>
         </is>
       </c>
       <c r="I66" t="inlineStr">
@@ -4027,7 +4027,7 @@
       </c>
       <c r="H67" t="inlineStr">
         <is>
-          <t>['Japan', 'Belgium']</t>
+          <t>['Belgium', 'Japan']</t>
         </is>
       </c>
       <c r="I67" t="inlineStr">
@@ -4174,7 +4174,7 @@
       <c r="G70" t="inlineStr"/>
       <c r="H70" t="inlineStr">
         <is>
-          <t>['Netherlands', 'Argentina']</t>
+          <t>['Argentina', 'Netherlands']</t>
         </is>
       </c>
       <c r="I70" t="inlineStr">
@@ -4272,7 +4272,7 @@
       <c r="G72" t="inlineStr"/>
       <c r="H72" t="inlineStr">
         <is>
-          <t>['Italy', 'Czech Republic']</t>
+          <t>['Czech Republic', 'Italy']</t>
         </is>
       </c>
       <c r="I72" t="inlineStr">
@@ -4665,7 +4665,7 @@
       <c r="G79" t="inlineStr"/>
       <c r="H79" t="inlineStr">
         <is>
-          <t>['South Korea', 'Switzerland']</t>
+          <t>['Switzerland', 'South Korea']</t>
         </is>
       </c>
       <c r="I79" t="inlineStr">
@@ -4724,7 +4724,7 @@
       </c>
       <c r="H80" t="inlineStr">
         <is>
-          <t>['France', 'Switzerland']</t>
+          <t>['Switzerland', 'France']</t>
         </is>
       </c>
       <c r="I80" t="inlineStr">
@@ -4871,7 +4871,7 @@
       <c r="G83" t="inlineStr"/>
       <c r="H83" t="inlineStr">
         <is>
-          <t>['South Korea', 'Argentina']</t>
+          <t>['Argentina', 'South Korea']</t>
         </is>
       </c>
       <c r="I83" t="inlineStr">
@@ -4930,7 +4930,7 @@
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>['Greece', 'Argentina']</t>
+          <t>['Argentina', 'Greece']</t>
         </is>
       </c>
       <c r="I84" t="inlineStr">
@@ -4989,7 +4989,7 @@
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>['South Korea', 'Argentina']</t>
+          <t>['Argentina', 'South Korea']</t>
         </is>
       </c>
       <c r="I85" t="inlineStr">
@@ -5038,7 +5038,7 @@
       <c r="G86" t="inlineStr"/>
       <c r="H86" t="inlineStr">
         <is>
-          <t>['Slovenia', 'United States']</t>
+          <t>['United States', 'Slovenia']</t>
         </is>
       </c>
       <c r="I86" t="inlineStr">
@@ -5097,7 +5097,7 @@
       </c>
       <c r="H87" t="inlineStr">
         <is>
-          <t>['Slovenia', 'England']</t>
+          <t>['England', 'Slovenia']</t>
         </is>
       </c>
       <c r="I87" t="inlineStr">
@@ -5156,7 +5156,7 @@
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>['England', 'United States']</t>
+          <t>['United States', 'England']</t>
         </is>
       </c>
       <c r="I88" t="inlineStr">
@@ -5205,7 +5205,7 @@
       <c r="G89" t="inlineStr"/>
       <c r="H89" t="inlineStr">
         <is>
-          <t>['Ghana', 'Germany']</t>
+          <t>['Germany', 'Ghana']</t>
         </is>
       </c>
       <c r="I89" t="inlineStr">
@@ -5254,7 +5254,7 @@
       <c r="G90" t="inlineStr"/>
       <c r="H90" t="inlineStr">
         <is>
-          <t>['Japan', 'Netherlands']</t>
+          <t>['Netherlands', 'Japan']</t>
         </is>
       </c>
       <c r="I90" t="inlineStr">
@@ -5460,7 +5460,7 @@
       <c r="G94" t="inlineStr"/>
       <c r="H94" t="inlineStr">
         <is>
-          <t>['Spain', 'Chile']</t>
+          <t>['Chile', 'Spain']</t>
         </is>
       </c>
       <c r="I94" t="inlineStr">
@@ -5607,7 +5607,7 @@
       <c r="G97" t="inlineStr"/>
       <c r="H97" t="inlineStr">
         <is>
-          <t>['Colombia', 'Ivory Coast']</t>
+          <t>['Ivory Coast', 'Colombia']</t>
         </is>
       </c>
       <c r="I97" t="inlineStr">
@@ -5666,7 +5666,7 @@
       </c>
       <c r="H98" t="inlineStr">
         <is>
-          <t>['Colombia', 'Greece']</t>
+          <t>['Greece', 'Colombia']</t>
         </is>
       </c>
       <c r="I98" t="inlineStr">
@@ -5725,7 +5725,7 @@
       </c>
       <c r="H99" t="inlineStr">
         <is>
-          <t>['Colombia', 'Ivory Coast']</t>
+          <t>['Ivory Coast', 'Colombia']</t>
         </is>
       </c>
       <c r="I99" t="inlineStr">
@@ -5784,7 +5784,7 @@
       </c>
       <c r="H100" t="inlineStr">
         <is>
-          <t>['Colombia', 'Greece']</t>
+          <t>['Greece', 'Colombia']</t>
         </is>
       </c>
       <c r="I100" t="inlineStr">
@@ -5833,7 +5833,7 @@
       <c r="G101" t="inlineStr"/>
       <c r="H101" t="inlineStr">
         <is>
-          <t>['Italy', 'Costa Rica']</t>
+          <t>['Costa Rica', 'Italy']</t>
         </is>
       </c>
       <c r="I101" t="inlineStr">
@@ -5892,7 +5892,7 @@
       </c>
       <c r="H102" t="inlineStr">
         <is>
-          <t>['Uruguay', 'Costa Rica']</t>
+          <t>['Costa Rica', 'Uruguay']</t>
         </is>
       </c>
       <c r="I102" t="inlineStr">
@@ -5941,7 +5941,7 @@
       <c r="G103" t="inlineStr"/>
       <c r="H103" t="inlineStr">
         <is>
-          <t>['France', 'Ecuador']</t>
+          <t>['Ecuador', 'France']</t>
         </is>
       </c>
       <c r="I103" t="inlineStr">
@@ -6000,7 +6000,7 @@
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>['France', 'Switzerland']</t>
+          <t>['Switzerland', 'France']</t>
         </is>
       </c>
       <c r="I104" t="inlineStr">
@@ -6049,7 +6049,7 @@
       <c r="G105" t="inlineStr"/>
       <c r="H105" t="inlineStr">
         <is>
-          <t>['Nigeria', 'Argentina']</t>
+          <t>['Argentina', 'Nigeria']</t>
         </is>
       </c>
       <c r="I105" t="inlineStr">
@@ -6147,7 +6147,7 @@
       <c r="G107" t="inlineStr"/>
       <c r="H107" t="inlineStr">
         <is>
-          <t>['Algeria', 'Belgium']</t>
+          <t>['Belgium', 'Algeria']</t>
         </is>
       </c>
       <c r="I107" t="inlineStr">
@@ -6265,7 +6265,7 @@
       </c>
       <c r="H109" t="inlineStr">
         <is>
-          <t>['Algeria', 'Belgium']</t>
+          <t>['Belgium', 'Algeria']</t>
         </is>
       </c>
       <c r="I109" t="inlineStr">
@@ -6461,7 +6461,7 @@
       <c r="G113" t="inlineStr"/>
       <c r="H113" t="inlineStr">
         <is>
-          <t>['Croatia', 'Nigeria']</t>
+          <t>['Nigeria', 'Croatia']</t>
         </is>
       </c>
       <c r="I113" t="inlineStr">
@@ -6520,7 +6520,7 @@
       </c>
       <c r="H114" t="inlineStr">
         <is>
-          <t>['Croatia', 'Argentina']</t>
+          <t>['Argentina', 'Croatia']</t>
         </is>
       </c>
       <c r="I114" t="inlineStr">
@@ -6579,7 +6579,7 @@
       </c>
       <c r="H115" t="inlineStr">
         <is>
-          <t>['Croatia', 'Nigeria']</t>
+          <t>['Nigeria', 'Croatia']</t>
         </is>
       </c>
       <c r="I115" t="inlineStr">
@@ -6638,7 +6638,7 @@
       </c>
       <c r="H116" t="inlineStr">
         <is>
-          <t>['Croatia', 'Argentina']</t>
+          <t>['Argentina', 'Croatia']</t>
         </is>
       </c>
       <c r="I116" t="inlineStr">
@@ -6687,7 +6687,7 @@
       <c r="G117" t="inlineStr"/>
       <c r="H117" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="I117" t="inlineStr">
@@ -6893,7 +6893,7 @@
       <c r="G121" t="inlineStr"/>
       <c r="H121" t="inlineStr">
         <is>
-          <t>['Japan', 'Senegal']</t>
+          <t>['Senegal', 'Japan']</t>
         </is>
       </c>
       <c r="I121" t="inlineStr">
@@ -7060,7 +7060,7 @@
       </c>
       <c r="H124" t="inlineStr">
         <is>
-          <t>['Senegal', 'Netherlands']</t>
+          <t>['Netherlands', 'Senegal']</t>
         </is>
       </c>
       <c r="I124" t="inlineStr">
@@ -7178,7 +7178,7 @@
       </c>
       <c r="H126" t="inlineStr">
         <is>
-          <t>['Senegal', 'Netherlands']</t>
+          <t>['Netherlands', 'Senegal']</t>
         </is>
       </c>
       <c r="I126" t="inlineStr">
@@ -7286,7 +7286,7 @@
       </c>
       <c r="H128" t="inlineStr">
         <is>
-          <t>['England', 'United States']</t>
+          <t>['United States', 'England']</t>
         </is>
       </c>
       <c r="I128" t="inlineStr">
@@ -7335,7 +7335,7 @@
       <c r="G129" t="inlineStr"/>
       <c r="H129" t="inlineStr">
         <is>
-          <t>['Poland', 'Argentina']</t>
+          <t>['Argentina', 'Poland']</t>
         </is>
       </c>
       <c r="I129" t="inlineStr">
@@ -7610,7 +7610,7 @@
       </c>
       <c r="H134" t="inlineStr">
         <is>
-          <t>['Spain', 'Germany']</t>
+          <t>['Germany', 'Spain']</t>
         </is>
       </c>
       <c r="I134" t="inlineStr">
@@ -7669,7 +7669,7 @@
       </c>
       <c r="H135" t="inlineStr">
         <is>
-          <t>['Japan', 'Spain']</t>
+          <t>['Spain', 'Japan']</t>
         </is>
       </c>
       <c r="I135" t="inlineStr">
@@ -7728,7 +7728,7 @@
       </c>
       <c r="H136" t="inlineStr">
         <is>
-          <t>['Japan', 'Costa Rica']</t>
+          <t>['Costa Rica', 'Japan']</t>
         </is>
       </c>
       <c r="I136" t="inlineStr">
@@ -7787,7 +7787,7 @@
       </c>
       <c r="H137" t="inlineStr">
         <is>
-          <t>['Japan', 'Spain']</t>
+          <t>['Spain', 'Japan']</t>
         </is>
       </c>
       <c r="I137" t="inlineStr">
@@ -7836,7 +7836,7 @@
       <c r="G138" t="inlineStr"/>
       <c r="H138" t="inlineStr">
         <is>
-          <t>['Croatia', 'Morocco']</t>
+          <t>['Morocco', 'Croatia']</t>
         </is>
       </c>
       <c r="I138" t="inlineStr">
@@ -7885,7 +7885,7 @@
       <c r="G139" t="inlineStr"/>
       <c r="H139" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="I139" t="inlineStr">
@@ -7944,7 +7944,7 @@
       </c>
       <c r="H140" t="inlineStr">
         <is>
-          <t>['Serbia', 'Brazil']</t>
+          <t>['Brazil', 'Serbia']</t>
         </is>
       </c>
       <c r="I140" t="inlineStr">
@@ -8003,7 +8003,7 @@
       </c>
       <c r="H141" t="inlineStr">
         <is>
-          <t>['Brazil', 'Switzerland']</t>
+          <t>['Switzerland', 'Brazil']</t>
         </is>
       </c>
       <c r="I141" t="inlineStr">

</xml_diff>